<commit_message>
Update to SCAR language
</commit_message>
<xml_diff>
--- a/app/config/tables/SCAR/forms/SCAR/SCAR.xlsx
+++ b/app/config/tables/SCAR/forms/SCAR/SCAR.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C0E218-7937-4F42-A144-8ADF33B7E577}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D9803B-9E72-4146-A236-4D77081EFBA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -206,9 +206,6 @@
     <t>Number of scar</t>
   </si>
   <si>
-    <t>Numero de sicatriz</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
@@ -399,6 +396,9 @@
   </si>
   <si>
     <t>Cicatrizes</t>
+  </si>
+  <si>
+    <t>Numero de cicatriz</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
@@ -792,13 +792,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>18</v>
@@ -809,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -825,7 +825,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,10 +833,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
         <v>121</v>
-      </c>
-      <c r="D5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -852,7 +852,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -863,15 +863,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -887,9 +887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +925,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>11</v>
@@ -976,10 +976,10 @@
         <v>44</v>
       </c>
       <c r="G5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" t="s">
         <v>110</v>
-      </c>
-      <c r="H5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1074,7 +1074,7 @@
         <v>57</v>
       </c>
       <c r="H15" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1100,30 +1100,30 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s">
         <v>59</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1131,13 +1131,13 @@
         <v>31</v>
       </c>
       <c r="F21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>67</v>
-      </c>
-      <c r="H21" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1155,7 +1155,7 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1168,10 +1168,10 @@
         <v>38</v>
       </c>
       <c r="G26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" t="s">
         <v>70</v>
-      </c>
-      <c r="H26" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" t="s">
         <v>50</v>
@@ -1196,7 +1196,7 @@
         <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
         <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G29" t="s">
         <v>53</v>
@@ -1226,13 +1226,13 @@
         <v>55</v>
       </c>
       <c r="F31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G31" t="s">
         <v>57</v>
       </c>
       <c r="H31" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1250,38 +1250,38 @@
         <v>38</v>
       </c>
       <c r="G34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34" t="s">
         <v>70</v>
-      </c>
-      <c r="H34" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G36" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -1289,13 +1289,13 @@
         <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G37" t="s">
+        <v>66</v>
+      </c>
+      <c r="H37" t="s">
         <v>67</v>
-      </c>
-      <c r="H37" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -1313,7 +1313,7 @@
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -1326,10 +1326,10 @@
         <v>38</v>
       </c>
       <c r="G42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H42" t="s">
         <v>79</v>
-      </c>
-      <c r="H42" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
         <v>48</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G43" t="s">
         <v>50</v>
@@ -1354,7 +1354,7 @@
         <v>34</v>
       </c>
       <c r="C44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -1365,7 +1365,7 @@
         <v>27</v>
       </c>
       <c r="F45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G45" t="s">
         <v>53</v>
@@ -1384,13 +1384,13 @@
         <v>55</v>
       </c>
       <c r="F47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G47" t="s">
         <v>57</v>
       </c>
       <c r="H47" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -1408,38 +1408,38 @@
         <v>38</v>
       </c>
       <c r="G50" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" t="s">
         <v>79</v>
-      </c>
-      <c r="H50" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G51" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G52" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
@@ -1447,13 +1447,13 @@
         <v>31</v>
       </c>
       <c r="F53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G53" t="s">
+        <v>66</v>
+      </c>
+      <c r="H53" t="s">
         <v>67</v>
-      </c>
-      <c r="H53" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>34</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>48</v>
       </c>
       <c r="F58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G58" t="s">
         <v>50</v>
@@ -1501,7 +1501,7 @@
         <v>34</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>27</v>
       </c>
       <c r="F60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G60" t="s">
         <v>53</v>
@@ -1531,13 +1531,13 @@
         <v>55</v>
       </c>
       <c r="F62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G62" t="s">
         <v>57</v>
       </c>
       <c r="H62" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -1555,38 +1555,38 @@
         <v>38</v>
       </c>
       <c r="G65" t="s">
+        <v>90</v>
+      </c>
+      <c r="H65" t="s">
         <v>91</v>
-      </c>
-      <c r="H65" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G66" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H66" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G67" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H67" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -1594,13 +1594,13 @@
         <v>31</v>
       </c>
       <c r="F68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G68" t="s">
+        <v>66</v>
+      </c>
+      <c r="H68" t="s">
         <v>67</v>
-      </c>
-      <c r="H68" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -1638,30 +1638,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
         <v>107</v>
-      </c>
-      <c r="B2" t="s">
-        <v>108</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1694,7 +1694,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
@@ -1754,10 +1754,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1769,10 +1769,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,7 +1784,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>30</v>
@@ -1893,10 +1893,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -1904,10 +1904,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -1915,10 +1915,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -1926,10 +1926,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
@@ -1981,7 +1981,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -1992,7 +1992,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
@@ -2025,7 +2025,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
@@ -2080,10 +2080,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -2091,10 +2091,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2102,10 +2102,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2113,10 +2113,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -2135,7 +2135,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
         <v>55</v>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
         <v>55</v>
@@ -2157,7 +2157,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
@@ -2179,10 +2179,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
         <v>55</v>

</xml_diff>